<commit_message>
Cambios en el controlador para subir excel e imágenes a la BD (sin resultado)
</commit_message>
<xml_diff>
--- a/public/plantillas/fichero_plantilla.xlsx
+++ b/public/plantillas/fichero_plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosloringrubio/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A919E04D-3C3E-8C4D-940F-2747ECD00F89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6503E0C8-10E0-EA43-91C8-11A7714F796E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="460" windowWidth="38640" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>id_cliente</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -34,44 +28,47 @@
     <t>email</t>
   </si>
   <si>
-    <t>email_verivied_at</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>remember_token</t>
-  </si>
-  <si>
-    <t>created_at</t>
-  </si>
-  <si>
-    <t>updated_at</t>
-  </si>
-  <si>
     <t>img_usuario</t>
   </si>
   <si>
     <t>cod_nivel</t>
   </si>
   <si>
-    <t>theme</t>
-  </si>
-  <si>
-    <t>collapse</t>
-  </si>
-  <si>
-    <t>val_timezone</t>
-  </si>
-  <si>
-    <t>last_login</t>
+    <t>manolo</t>
+  </si>
+  <si>
+    <t>manolo.jpg</t>
+  </si>
+  <si>
+    <t>pepe</t>
+  </si>
+  <si>
+    <t>pepe.jpg</t>
+  </si>
+  <si>
+    <t>paco</t>
+  </si>
+  <si>
+    <t>paco.jpg</t>
+  </si>
+  <si>
+    <t>manolo33@manolo.com</t>
+  </si>
+  <si>
+    <t>pepe33@pepe.com</t>
+  </si>
+  <si>
+    <t>paco33@paco.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -81,6 +78,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -101,14 +104,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,34 +417,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" customWidth="1"/>
-    <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" bestFit="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,41 +451,67 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{C9F4EBEE-EFAE-4D63-A534-E88314D55DB5}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{A463E873-7FD3-4877-9473-AB9B088772E5}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{2F02F967-746E-4EE1-B0EB-66839E2C1851}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Mejora de la estética del wizard
</commit_message>
<xml_diff>
--- a/public/plantillas/fichero_plantilla.xlsx
+++ b/public/plantillas/fichero_plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosloringrubio/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6503E0C8-10E0-EA43-91C8-11A7714F796E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43421612-47D3-A944-AB70-33AFB83E8774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="460" windowWidth="38640" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>name</t>
   </si>
@@ -35,33 +35,6 @@
   </si>
   <si>
     <t>cod_nivel</t>
-  </si>
-  <si>
-    <t>manolo</t>
-  </si>
-  <si>
-    <t>manolo.jpg</t>
-  </si>
-  <si>
-    <t>pepe</t>
-  </si>
-  <si>
-    <t>pepe.jpg</t>
-  </si>
-  <si>
-    <t>paco</t>
-  </si>
-  <si>
-    <t>paco.jpg</t>
-  </si>
-  <si>
-    <t>manolo33@manolo.com</t>
-  </si>
-  <si>
-    <t>pepe33@pepe.com</t>
-  </si>
-  <si>
-    <t>paco33@paco.com</t>
   </si>
 </sst>
 </file>
@@ -420,7 +393,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -455,63 +428,16 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{C9F4EBEE-EFAE-4D63-A534-E88314D55DB5}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{A463E873-7FD3-4877-9473-AB9B088772E5}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{2F02F967-746E-4EE1-B0EB-66839E2C1851}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>